<commit_message>
Updated Excel file and minor code changes
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkinn\OneDrive\Desktop\Revature\Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAED1258-32ED-4E75-939B-AE297D1BD9F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE029F83-3220-44BC-853D-4350462B8C5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39270" yWindow="1470" windowWidth="17085" windowHeight="12465" xr2:uid="{AB93EBE2-CCBE-471C-A8AA-AFE999001AAE}"/>
+    <workbookView xWindow="26715" yWindow="1170" windowWidth="17085" windowHeight="12465" xr2:uid="{AB93EBE2-CCBE-471C-A8AA-AFE999001AAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>Employee Requirements</t>
   </si>
@@ -109,13 +109,61 @@
   </si>
   <si>
     <t>not completed</t>
+  </si>
+  <si>
+    <t>Technologies</t>
+  </si>
+  <si>
+    <t>Used?</t>
+  </si>
+  <si>
+    <t>Java 1.8</t>
+  </si>
+  <si>
+    <t>Servlets</t>
+  </si>
+  <si>
+    <t>JDBC</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>PL/SQL</t>
+  </si>
+  <si>
+    <t>HTML/CSS</t>
+  </si>
+  <si>
+    <t>Bootstrap</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>AJAX</t>
+  </si>
+  <si>
+    <t>Junit</t>
+  </si>
+  <si>
+    <t>Java Mail</t>
+  </si>
+  <si>
+    <t>Log4j</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,13 +179,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -152,9 +226,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,132 +554,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F42B075-C3A1-4A3B-A7E4-02B3C29E8A6E}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="4"/>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D10" s="4"/>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -602,7 +781,7 @@
       <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -610,7 +789,7 @@
       <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -623,7 +802,7 @@
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -631,7 +810,7 @@
       <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -639,7 +818,7 @@
       <c r="A23" t="s">
         <v>17</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -647,7 +826,7 @@
       <c r="A24" t="s">
         <v>20</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -655,7 +834,7 @@
       <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>